<commit_message>
added northwind star schema flat files
</commit_message>
<xml_diff>
--- a/LabFiles/StarterFiles/NorthwindFlatFiles/Customers.xlsx
+++ b/LabFiles/StarterFiles/NorthwindFlatFiles/Customers.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\content-writing\working-with-power-bi\LabFiles - Copy\StarterFiles\NorthwindFlatFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\courses\pluralsight_deloitte_powerbi\LabFiles\StarterFiles\NorthwindFlatFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26AC4B98-A196-44A6-A1B2-093CE911BA98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F3FD72-2457-4552-A2C8-6B00EF7E489E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67980" yWindow="780" windowWidth="28800" windowHeight="11010" xr2:uid="{0723FDEA-B9FD-4CBD-8360-CB6DDDA96F62}"/>
+    <workbookView xWindow="38280" yWindow="6855" windowWidth="29040" windowHeight="15720" xr2:uid="{0723FDEA-B9FD-4CBD-8360-CB6DDDA96F62}"/>
   </bookViews>
   <sheets>
-    <sheet name="Customers" sheetId="1" r:id="rId1"/>
+    <sheet name="Customers" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2417,7 +2417,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1E5EF3B-7EBC-43DB-8C84-687CF71E2C2A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2A60F9C-CE6E-4CDD-A37A-7139B6977001}">
   <dimension ref="A1:K92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>